<commit_message>
Initial layout of the model
</commit_message>
<xml_diff>
--- a/Data/Interchange.xlsx
+++ b/Data/Interchange.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Bus2_import</t>
+  </si>
+  <si>
+    <t>Bus3_import</t>
+  </si>
+  <si>
+    <t>Bus</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -373,7 +379,7 @@
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -383,8 +389,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -394,8 +403,11 @@
       <c r="C2">
         <v>90</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -404,6 +416,23 @@
       </c>
       <c r="C3">
         <v>100</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>